<commit_message>
Added results wt.rep, wt.par, wt.pin, for ed richardson to look at
</commit_message>
<xml_diff>
--- a/GrowthIncrement.xlsx
+++ b/GrowthIncrement.xlsx
@@ -26,10 +26,13 @@
     <definedName name="Weight">Sheet1!$F$5:$O$5</definedName>
     <definedName name="winf">Sheet1!$B$12</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
@@ -309,6 +312,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -386,34 +394,34 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.0453847248716039</c:v>
+                  <c:v>0.0454622439359603</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.603515697972024</c:v>
+                  <c:v>0.669415352021826</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.584599876495278</c:v>
+                  <c:v>1.894244797335531</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.922437432826345</c:v>
+                  <c:v>3.125082690425185</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.1452125665368</c:v>
+                  <c:v>5.834539512691924</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.980687485441034</c:v>
+                  <c:v>8.13263167495903</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.580038455070104</c:v>
+                  <c:v>7.294801303082293</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.816010611397069</c:v>
+                  <c:v>6.888379643690801</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.45032984477364</c:v>
+                  <c:v>7.894829251984895</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.192237554070016</c:v>
+                  <c:v>9.446644170873023</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -474,34 +482,34 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.0320715203960037</c:v>
+                  <c:v>0.0424610311953934</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.803128974496083</c:v>
+                  <c:v>0.69352114021184</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.934363394259772</c:v>
+                  <c:v>1.926037651025874</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.706141715873408</c:v>
+                  <c:v>3.230720445727253</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.386945076593036</c:v>
+                  <c:v>4.636256399217403</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.565918284230909</c:v>
+                  <c:v>7.108059311349479</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.169767006210578</c:v>
+                  <c:v>9.40140008794256</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.304984392532988</c:v>
+                  <c:v>8.104442794197174</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.517434888769566</c:v>
+                  <c:v>7.425971611637797</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.813881676198193</c:v>
+                  <c:v>8.237918086846111</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -562,34 +570,34 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.0329216545091727</c:v>
+                  <c:v>0.0359037766021993</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.794183689154848</c:v>
+                  <c:v>0.698275807077202</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.883876349368662</c:v>
+                  <c:v>1.906711635115407</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.854257664942493</c:v>
+                  <c:v>3.621464287255134</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.989437419988723</c:v>
+                  <c:v>5.132499264313025</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.900393601169895</c:v>
+                  <c:v>6.342121919796035</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.77740391979069</c:v>
+                  <c:v>7.417540666357976</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.694183749133859</c:v>
+                  <c:v>7.335535559288341</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.480177684649445</c:v>
+                  <c:v>8.021872576806444</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.253835753055934</c:v>
+                  <c:v>10.45359910045721</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -650,34 +658,34 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.0372294685205424</c:v>
+                  <c:v>0.0470265017441749</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.506313410459186</c:v>
+                  <c:v>0.586472090435572</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.205539902668225</c:v>
+                  <c:v>2.10305874847437</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.218442593320868</c:v>
+                  <c:v>3.575147032368101</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.150538405573391</c:v>
+                  <c:v>5.090743992557325</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.877494646546284</c:v>
+                  <c:v>6.542317296325518</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.16391993910648</c:v>
+                  <c:v>7.452063277589882</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.43563579919011</c:v>
+                  <c:v>8.189597753865854</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.146987623166451</c:v>
+                  <c:v>7.834012306824014</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.826643057399023</c:v>
+                  <c:v>8.372952325494752</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -738,34 +746,34 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.0444802315509194</c:v>
+                  <c:v>0.045027260881054</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.626626792043335</c:v>
+                  <c:v>0.805727835449099</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.903609043177162</c:v>
+                  <c:v>2.3005100527183</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.95322095150363</c:v>
+                  <c:v>3.557720150944418</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.619624787065878</c:v>
+                  <c:v>5.637833708075231</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.664353632774953</c:v>
+                  <c:v>5.338920235063702</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.483029034474208</c:v>
+                  <c:v>7.173942509351044</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.741596018760457</c:v>
+                  <c:v>7.49070411635641</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.853527613273047</c:v>
+                  <c:v>9.098998327795375</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.035755988177907</c:v>
+                  <c:v>9.76697208808675</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -826,34 +834,34 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.033396477098893</c:v>
+                  <c:v>0.0403390069954073</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.722961204231001</c:v>
+                  <c:v>0.740298197602994</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.888426074755074</c:v>
+                  <c:v>2.306807393686856</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.373233419486096</c:v>
+                  <c:v>4.026872165474523</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.375461008624674</c:v>
+                  <c:v>5.173492621537532</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.60972360587503</c:v>
+                  <c:v>7.04352564441832</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.655716631714237</c:v>
+                  <c:v>6.250601555660286</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.40051331161182</c:v>
+                  <c:v>7.879372079568353</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.286497644401634</c:v>
+                  <c:v>8.123925691090903</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.298580397993101</c:v>
+                  <c:v>9.40691895032627</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -868,11 +876,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2137591912"/>
-        <c:axId val="-2137595224"/>
+        <c:axId val="-2133489960"/>
+        <c:axId val="-2133486808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2137591912"/>
+        <c:axId val="-2133489960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -881,12 +889,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2137595224"/>
+        <c:crossAx val="-2133486808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2137595224"/>
+        <c:axId val="-2133486808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -897,7 +905,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2137591912"/>
+        <c:crossAx val="-2133489960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -924,15 +932,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1279,7 +1287,7 @@
   <dimension ref="A1:Q76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1495,7 +1503,7 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
@@ -1790,47 +1798,47 @@
       </c>
       <c r="F12" s="1">
         <f t="shared" ref="F12:O12" ca="1" si="7">winf*(1-EXP(-k*(Age-to)))^b*EXP(sigma_y*$Q12+sigma_c*F36+F58)</f>
-        <v>4.5384724871603943E-2</v>
+        <v>4.5462243935960295E-2</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>0.60351569797202431</v>
+        <v>0.66941535202182589</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>1.5845998764952778</v>
+        <v>1.8942447973355308</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>3.9224374328263449</v>
+        <v>3.1250826904251849</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>5.1452125665367996</v>
+        <v>5.8345395126919239</v>
       </c>
       <c r="K12" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>5.9806874854410346</v>
+        <v>8.1326316749590308</v>
       </c>
       <c r="L12" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>5.5800384550701043</v>
+        <v>7.2948013030822931</v>
       </c>
       <c r="M12" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>6.8160106113970693</v>
+        <v>6.8883796436908016</v>
       </c>
       <c r="N12" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>7.4503298447736395</v>
+        <v>7.8948292519848948</v>
       </c>
       <c r="O12" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>9.192237554070017</v>
+        <v>9.4466441708730233</v>
       </c>
       <c r="Q12" s="3">
         <f ca="1">_xlfn.NORM.INV(RAND(),0,1)</f>
-        <v>-0.48450039609713685</v>
+        <v>-0.53991653912587068</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1839,47 +1847,47 @@
       </c>
       <c r="F13" s="1">
         <f t="shared" ref="F13:F30" ca="1" si="8">winf*(1-EXP(-k*(Age-to)))^b*EXP(sigma_y*$Q13+sigma_c*F37+F59)</f>
-        <v>3.2071520396003715E-2</v>
+        <v>4.2461031195393392E-2</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" ref="G13:G30" ca="1" si="9">F12+winf*EXP(-b*delta*k-(Age-1)*b*k)*((EXP(delta*k+(Age-1)*k)-EXP(k*to))^b-EXP(b*delta*k)*(EXP((Age-1)*k)-EXP(k*to))^b)*EXP(sigma_y*$Q12+sigma_c*G37+G59)</f>
-        <v>0.80312897449608323</v>
+        <v>0.69352114021184019</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" ref="H13:H30" ca="1" si="10">G12+winf*EXP(-b*delta*k-(Age-1)*b*k)*((EXP(delta*k+(Age-1)*k)-EXP(k*to))^b-EXP(b*delta*k)*(EXP((Age-1)*k)-EXP(k*to))^b)*EXP(sigma_y*$Q12+sigma_c*H37+H59)</f>
-        <v>1.9343633942597722</v>
+        <v>1.9260376510258741</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" ref="I13:I30" ca="1" si="11">H12+winf*EXP(-b*delta*k-(Age-1)*b*k)*((EXP(delta*k+(Age-1)*k)-EXP(k*to))^b-EXP(b*delta*k)*(EXP((Age-1)*k)-EXP(k*to))^b)*EXP(sigma_y*$Q12+sigma_c*I37+I59)</f>
-        <v>2.7061417158734078</v>
+        <v>3.2307204457272536</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" ref="J13:J30" ca="1" si="12">I12+winf*EXP(-b*delta*k-(Age-1)*b*k)*((EXP(delta*k+(Age-1)*k)-EXP(k*to))^b-EXP(b*delta*k)*(EXP((Age-1)*k)-EXP(k*to))^b)*EXP(sigma_y*$Q12+sigma_c*J37+J59)</f>
-        <v>5.3869450765930358</v>
+        <v>4.6362563992174035</v>
       </c>
       <c r="K13" s="1">
         <f t="shared" ref="K13:K30" ca="1" si="13">J12+winf*EXP(-b*delta*k-(Age-1)*b*k)*((EXP(delta*k+(Age-1)*k)-EXP(k*to))^b-EXP(b*delta*k)*(EXP((Age-1)*k)-EXP(k*to))^b)*EXP(sigma_y*$Q12+sigma_c*K37+K59)</f>
-        <v>6.565918284230909</v>
+        <v>7.1080593113494785</v>
       </c>
       <c r="L13" s="1">
         <f t="shared" ref="L13:L30" ca="1" si="14">K12+winf*EXP(-b*delta*k-(Age-1)*b*k)*((EXP(delta*k+(Age-1)*k)-EXP(k*to))^b-EXP(b*delta*k)*(EXP((Age-1)*k)-EXP(k*to))^b)*EXP(sigma_y*$Q12+sigma_c*L37+L59)</f>
-        <v>7.1697670062105781</v>
+        <v>9.4014000879425605</v>
       </c>
       <c r="M13" s="1">
         <f t="shared" ref="M13:M30" ca="1" si="15">L12+winf*EXP(-b*delta*k-(Age-1)*b*k)*((EXP(delta*k+(Age-1)*k)-EXP(k*to))^b-EXP(b*delta*k)*(EXP((Age-1)*k)-EXP(k*to))^b)*EXP(sigma_y*$Q12+sigma_c*M37+M59)</f>
-        <v>6.3049843925329876</v>
+        <v>8.1044427941971744</v>
       </c>
       <c r="N13" s="1">
         <f t="shared" ref="N13:N30" ca="1" si="16">M12+winf*EXP(-b*delta*k-(Age-1)*b*k)*((EXP(delta*k+(Age-1)*k)-EXP(k*to))^b-EXP(b*delta*k)*(EXP((Age-1)*k)-EXP(k*to))^b)*EXP(sigma_y*$Q12+sigma_c*N37+N59)</f>
-        <v>7.5174348887695661</v>
+        <v>7.425971611637797</v>
       </c>
       <c r="O13" s="1">
         <f t="shared" ref="O13:O30" ca="1" si="17">N12+winf*EXP(-b*delta*k-(Age-1)*b*k)*((EXP(delta*k+(Age-1)*k)-EXP(k*to))^b-EXP(b*delta*k)*(EXP((Age-1)*k)-EXP(k*to))^b)*EXP(sigma_y*$Q12+sigma_c*O37+O59)</f>
-        <v>7.8138816761981928</v>
+        <v>8.2379180868461113</v>
       </c>
       <c r="Q13" s="3">
         <f t="shared" ref="Q13:Q30" ca="1" si="18">_xlfn.NORM.INV(RAND(),0,1)</f>
-        <v>-0.26780985020460762</v>
+        <v>-0.27026944423785842</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1888,47 +1896,47 @@
       </c>
       <c r="F14" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>4.7859397669173603E-2</v>
+        <v>4.2248370453548893E-2</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0.55961614301643681</v>
+        <v>0.68219388131405723</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>2.3376191764906809</v>
+        <v>2.0994781484370044</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>3.4910462359427443</v>
+        <v>3.5603025276467379</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>3.9234568481347534</v>
+        <v>4.5851811965472828</v>
       </c>
       <c r="K14" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>6.8449043353129913</v>
+        <v>5.8681566535064391</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>7.4134263526775737</v>
+        <v>8.3816224041622487</v>
       </c>
       <c r="M14" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>7.9403203663008162</v>
+        <v>10.401621317563807</v>
       </c>
       <c r="N14" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>6.7618056265340156</v>
+        <v>8.5984020468205973</v>
       </c>
       <c r="O14" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>7.8928443738384351</v>
+        <v>7.8042540187191083</v>
       </c>
       <c r="Q14" s="3">
         <f t="shared" ca="1" si="18"/>
-        <v>1.0340245901108764</v>
+        <v>-0.60200142001017087</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1937,47 +1945,47 @@
       </c>
       <c r="F15" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>3.9465866102664206E-2</v>
+        <v>4.0085513621324356E-2</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0.72776931746639628</v>
+        <v>0.60129703975553894</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>1.6068572605836204</v>
+        <v>2.0501130130265341</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>4.2324784246885816</v>
+        <v>3.9340214512507226</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>5.3669841094103949</v>
+        <v>5.3332520763293463</v>
       </c>
       <c r="K15" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>5.1507145733917588</v>
+        <v>5.7974971858588615</v>
       </c>
       <c r="L15" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>7.9661550333231119</v>
+        <v>6.8614600779483874</v>
       </c>
       <c r="M15" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>8.2820577072876844</v>
+        <v>9.3092529187887081</v>
       </c>
       <c r="N15" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>8.5503227911888509</v>
+        <v>11.180274261511844</v>
       </c>
       <c r="O15" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>7.1687871552773652</v>
+        <v>9.0746826036886379</v>
       </c>
       <c r="Q15" s="3">
         <f t="shared" ca="1" si="18"/>
-        <v>0.319777639669518</v>
+        <v>-1.998038519916699</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1986,47 +1994,47 @@
       </c>
       <c r="F16" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>4.8935198580374192E-2</v>
+        <v>4.0895700892695605E-2</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0.66545737860463938</v>
+        <v>0.66270321986945857</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>2.3099906774600325</v>
+        <v>1.986584538999657</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>2.9716902226619251</v>
+        <v>3.6484177908127249</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>6.4895642404485283</v>
+        <v>5.2156944919958281</v>
       </c>
       <c r="K16" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>6.8223271025844383</v>
+        <v>6.5209778531936351</v>
       </c>
       <c r="L16" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>6.025507723657249</v>
+        <v>6.65611096080913</v>
       </c>
       <c r="M16" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>8.8687493965431425</v>
+        <v>7.5939167799668512</v>
       </c>
       <c r="N16" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>8.8041390451733665</v>
+        <v>9.9468253252225427</v>
       </c>
       <c r="O16" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>8.9438407577647894</v>
+        <v>11.708900794823331</v>
       </c>
       <c r="Q16" s="3">
         <f t="shared" ca="1" si="18"/>
-        <v>-0.49604648626583897</v>
+        <v>-0.81083759739832462</v>
       </c>
     </row>
     <row r="17" spans="5:17">
@@ -2035,47 +2043,47 @@
       </c>
       <c r="F17" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>3.2921654509172713E-2</v>
+        <v>3.5903776602199317E-2</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0.79418368915484849</v>
+        <v>0.69827580707720227</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>1.8838763493686617</v>
+        <v>1.9067116351154074</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>3.8542576649424927</v>
+        <v>3.6214642872551339</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>3.9894374199887226</v>
+        <v>5.1324992643130258</v>
       </c>
       <c r="K17" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>7.9003936011698954</v>
+        <v>6.3421219197960346</v>
       </c>
       <c r="L17" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>7.7774039197906895</v>
+        <v>7.4175406663579757</v>
       </c>
       <c r="M17" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>6.6941837491338596</v>
+        <v>7.3355355592883411</v>
       </c>
       <c r="N17" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>9.4801776846494459</v>
+        <v>8.0218725768064445</v>
       </c>
       <c r="O17" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>9.2538357530559345</v>
+        <v>10.453599100457209</v>
       </c>
       <c r="Q17" s="3">
         <f t="shared" ca="1" si="18"/>
-        <v>-1.1974542408412086</v>
+        <v>-0.89257288258082701</v>
       </c>
     </row>
     <row r="18" spans="5:17">
@@ -2084,47 +2092,47 @@
       </c>
       <c r="F18" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>3.7229468520542375E-2</v>
+        <v>4.7026501744174928E-2</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0.50631341045918643</v>
+        <v>0.58647209043557247</v>
       </c>
       <c r="H18" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>2.205539902668225</v>
+        <v>2.103058748474369</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>3.2184425933208685</v>
+        <v>3.5751470323681014</v>
       </c>
       <c r="J18" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>5.1505384055733909</v>
+        <v>5.0907439925573259</v>
       </c>
       <c r="K18" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>4.8774946465462836</v>
+        <v>6.5423172963255176</v>
       </c>
       <c r="L18" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>9.1639199391064814</v>
+        <v>7.4520632775898825</v>
       </c>
       <c r="M18" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>8.4356357991901092</v>
+        <v>8.1895977538658542</v>
       </c>
       <c r="N18" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>7.1469876231664511</v>
+        <v>7.8340123068240137</v>
       </c>
       <c r="O18" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>9.8266430573990231</v>
+        <v>8.3729523254947527</v>
       </c>
       <c r="Q18" s="3">
         <f t="shared" ca="1" si="18"/>
-        <v>0.66026720854475274</v>
+        <v>0.43499293747852208</v>
       </c>
     </row>
     <row r="19" spans="5:17">
@@ -2133,47 +2141,47 @@
       </c>
       <c r="F19" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>3.8895054990729275E-2</v>
+        <v>4.5290988143570965E-2</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0.64262889528989953</v>
+        <v>0.74313228991245928</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>1.7892883311046983</v>
+        <v>1.6708760291035405</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>4.0515670433869397</v>
+        <v>3.6326461223291262</v>
       </c>
       <c r="J19" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>4.6810879339492537</v>
+        <v>4.8980279408517413</v>
       </c>
       <c r="K19" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>6.629623599684189</v>
+        <v>6.5106182401456625</v>
       </c>
       <c r="L19" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>5.7739131620905066</v>
+        <v>7.7760576650508746</v>
       </c>
       <c r="M19" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>10.231246596612293</v>
+        <v>8.0867317616151464</v>
       </c>
       <c r="N19" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>9.0336146026785329</v>
+        <v>8.6309647452318856</v>
       </c>
       <c r="O19" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>7.506614495872034</v>
+        <v>8.1998338731694247</v>
       </c>
       <c r="Q19" s="3">
         <f t="shared" ca="1" si="18"/>
-        <v>-1.1015159267095591</v>
+        <v>0.84137233243473908</v>
       </c>
     </row>
     <row r="20" spans="5:17">
@@ -2182,47 +2190,47 @@
       </c>
       <c r="F20" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>4.8837887805348833E-2</v>
+        <v>4.6650158242258419E-2</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0.59830056372183626</v>
+        <v>0.68369465402078</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>1.6522069360369251</v>
+        <v>2.2388749391600902</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>3.2253244133387189</v>
+        <v>2.9661111691881077</v>
       </c>
       <c r="J20" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>5.4790986726212747</v>
+        <v>5.1524256369625663</v>
       </c>
       <c r="K20" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>5.8099150311971801</v>
+        <v>5.9341631663263392</v>
       </c>
       <c r="L20" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>7.6007955893189632</v>
+        <v>7.6511553334673286</v>
       </c>
       <c r="M20" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>6.2801019533693498</v>
+        <v>8.7655587648863573</v>
       </c>
       <c r="N20" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>10.975309100125045</v>
+        <v>8.6412558066474023</v>
       </c>
       <c r="O20" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>9.5051782313089745</v>
+        <v>9.1248644126063443</v>
       </c>
       <c r="Q20" s="3">
         <f t="shared" ca="1" si="18"/>
-        <v>2.1177093090924695</v>
+        <v>1.6574032309558664</v>
       </c>
     </row>
     <row r="21" spans="5:17">
@@ -2231,47 +2239,47 @@
       </c>
       <c r="F21" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>3.919834152405581E-2</v>
+        <v>4.5227176878925447E-2</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0.75580113716087827</v>
+        <v>0.78350598506932789</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>2.2342033887341461</v>
+        <v>2.0549082150449225</v>
       </c>
       <c r="I21" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>3.4308640908526047</v>
+        <v>3.8753426321843207</v>
       </c>
       <c r="J21" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>4.8280408031386939</v>
+        <v>4.2918626194806864</v>
       </c>
       <c r="K21" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>7.4841742835542124</v>
+        <v>6.3894743717285092</v>
       </c>
       <c r="L21" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>7.0678588769175157</v>
+        <v>6.7233080093681137</v>
       </c>
       <c r="M21" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>8.3203010784381899</v>
+        <v>8.3201001323052175</v>
       </c>
       <c r="N21" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>6.7993708614613677</v>
+        <v>9.388749689990842</v>
       </c>
       <c r="O21" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>11.49629473881266</v>
+        <v>9.1400938022446319</v>
       </c>
       <c r="Q21" s="3">
         <f t="shared" ca="1" si="18"/>
-        <v>8.522634702868441E-2</v>
+        <v>-0.49400040073600093</v>
       </c>
     </row>
     <row r="22" spans="5:17">
@@ -2280,47 +2288,47 @@
       </c>
       <c r="F22" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>4.4480231550919361E-2</v>
+        <v>4.5027260881054028E-2</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0.62662679204333538</v>
+        <v>0.80572783544909954</v>
       </c>
       <c r="H22" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>1.9036090431771622</v>
+        <v>2.3005100527182991</v>
       </c>
       <c r="I22" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>3.9532209515036305</v>
+        <v>3.5577201509444185</v>
       </c>
       <c r="J22" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>4.6196247870658782</v>
+        <v>5.637833708075231</v>
       </c>
       <c r="K22" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>5.6643536327749535</v>
+        <v>5.3389202350637017</v>
       </c>
       <c r="L22" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>8.4830290344742085</v>
+        <v>7.1739425093510443</v>
       </c>
       <c r="M22" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>7.7415960187604567</v>
+        <v>7.4907041163564099</v>
       </c>
       <c r="N22" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>8.853527613273048</v>
+        <v>9.0989983277953748</v>
       </c>
       <c r="O22" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>7.0357559881779066</v>
+        <v>9.7669720880867494</v>
       </c>
       <c r="Q22" s="3">
         <f t="shared" ca="1" si="18"/>
-        <v>0.39592766720882094</v>
+        <v>1.9654029175184937</v>
       </c>
     </row>
     <row r="23" spans="5:17">
@@ -2329,47 +2337,47 @@
       </c>
       <c r="F23" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>3.3396477098893054E-2</v>
+        <v>4.033900699540735E-2</v>
       </c>
       <c r="G23" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0.72296120423100085</v>
+        <v>0.74029819760299409</v>
       </c>
       <c r="H23" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>1.8884260747550745</v>
+        <v>2.3068073936868565</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>3.3732334194860965</v>
+        <v>4.0268721654745239</v>
       </c>
       <c r="J23" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>5.3754610086246748</v>
+        <v>5.1734926215375321</v>
       </c>
       <c r="K23" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>5.6097236058750299</v>
+        <v>7.0435256444183203</v>
       </c>
       <c r="L23" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>6.6557166317142373</v>
+        <v>6.2506015556602863</v>
       </c>
       <c r="M23" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>9.4005133116118191</v>
+        <v>7.8793720795683528</v>
       </c>
       <c r="N23" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>8.2864976444016349</v>
+        <v>8.1239256910909035</v>
       </c>
       <c r="O23" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>9.298580397993101</v>
+        <v>9.4069189503262702</v>
       </c>
       <c r="Q23" s="3">
         <f t="shared" ca="1" si="18"/>
-        <v>-1.3378331943197141</v>
+        <v>-9.1746306184397497E-2</v>
       </c>
     </row>
     <row r="24" spans="5:17">
@@ -2378,47 +2386,47 @@
       </c>
       <c r="F24" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>4.3674287273772656E-2</v>
+        <v>4.766590405821889E-2</v>
       </c>
       <c r="G24" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0.55072722138417463</v>
+        <v>0.67437089356970914</v>
       </c>
       <c r="H24" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>1.8626776515184695</v>
+        <v>2.0211385879388315</v>
       </c>
       <c r="I24" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>3.0487721042526195</v>
+        <v>3.9454481708281612</v>
       </c>
       <c r="J24" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>4.4413630792850949</v>
+        <v>5.6601678293593238</v>
       </c>
       <c r="K24" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>6.426164856806329</v>
+        <v>6.3967241967509612</v>
       </c>
       <c r="L24" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>6.2654335789825932</v>
+        <v>8.1419865297082072</v>
       </c>
       <c r="M24" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>7.2771556230918337</v>
+        <v>6.9538378809361472</v>
       </c>
       <c r="N24" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>10.111555932477259</v>
+        <v>8.4755360002484181</v>
       </c>
       <c r="O24" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>8.7593523000387492</v>
+        <v>8.6094038461004168</v>
       </c>
       <c r="Q24" s="3">
         <f t="shared" ca="1" si="18"/>
-        <v>0.51857090135503037</v>
+        <v>0.21344972429045383</v>
       </c>
     </row>
     <row r="25" spans="5:17">
@@ -2427,47 +2435,47 @@
       </c>
       <c r="F25" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>3.5699250865368286E-2</v>
+        <v>3.9275586329591952E-2</v>
       </c>
       <c r="G25" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0.74414647957579316</v>
+        <v>0.70962632553361182</v>
       </c>
       <c r="H25" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>1.9588314127710671</v>
+        <v>2.1653642781361788</v>
       </c>
       <c r="I25" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>3.4179436220286696</v>
+        <v>3.5696761829731067</v>
       </c>
       <c r="J25" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>4.3068818388583034</v>
+        <v>5.4259659012474817</v>
       </c>
       <c r="K25" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>5.502529098954148</v>
+        <v>7.0812377034644785</v>
       </c>
       <c r="L25" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>7.4977128614770416</v>
+        <v>7.4532417375340394</v>
       </c>
       <c r="M25" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>6.8886364152349779</v>
+        <v>9.1345918195744815</v>
       </c>
       <c r="N25" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>7.700265758404278</v>
+        <v>7.4075040417306734</v>
       </c>
       <c r="O25" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>10.58645151336593</v>
+        <v>8.8800500685680017</v>
       </c>
       <c r="Q25" s="3">
         <f t="shared" ca="1" si="18"/>
-        <v>-0.80644901383950363</v>
+        <v>-0.42374105375929605</v>
       </c>
     </row>
     <row r="26" spans="5:17">
@@ -2476,47 +2484,47 @@
       </c>
       <c r="F26" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>3.5341018365518229E-2</v>
+        <v>5.0386588974221477E-2</v>
       </c>
       <c r="G26" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0.61729245230646601</v>
+        <v>0.67183099568821414</v>
       </c>
       <c r="H26" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>2.0620749652222528</v>
+        <v>2.0582427961741456</v>
       </c>
       <c r="I26" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>3.4375766758881676</v>
+        <v>3.8481948471498564</v>
       </c>
       <c r="J26" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>4.8732126965691513</v>
+        <v>5.1994662652609254</v>
       </c>
       <c r="K26" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>5.3100386827012169</v>
+        <v>7.131650584518292</v>
       </c>
       <c r="L26" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>6.2909441113773603</v>
+        <v>8.1249920171693137</v>
       </c>
       <c r="M26" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>8.1207881719857422</v>
+        <v>8.2029266782944283</v>
       </c>
       <c r="N26" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>7.3676280909350131</v>
+        <v>9.8531262509688045</v>
       </c>
       <c r="O26" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>7.9649991451642697</v>
+        <v>7.7674618036039762</v>
       </c>
       <c r="Q26" s="3">
         <f t="shared" ca="1" si="18"/>
-        <v>0.1539661749628064</v>
+        <v>-1.5212789037653103</v>
       </c>
     </row>
     <row r="27" spans="5:17">
@@ -2525,47 +2533,47 @@
       </c>
       <c r="F27" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>4.3169391964696269E-2</v>
+        <v>4.6095047663951838E-2</v>
       </c>
       <c r="G27" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0.63608956378249837</v>
+        <v>0.82446573834024905</v>
       </c>
       <c r="H27" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>1.8202126962697143</v>
+        <v>1.896240750605354</v>
       </c>
       <c r="I27" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>3.5304353435491911</v>
+        <v>3.5707686812938215</v>
       </c>
       <c r="J27" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>4.9693672530233286</v>
+        <v>5.2611938308181712</v>
       </c>
       <c r="K27" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>5.943834498884482</v>
+        <v>6.5642300334399772</v>
       </c>
       <c r="L27" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>6.2128670143081761</v>
+        <v>8.1337054333873304</v>
       </c>
       <c r="M27" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>6.8889216081203895</v>
+        <v>8.9408379583063233</v>
       </c>
       <c r="N27" s="1">
-        <f t="shared" ca="1" si="16"/>
-        <v>8.6912338454928602</v>
+        <f ca="1">M26+winf*EXP(-b*delta*k-(Age-1)*b*k)*((EXP(delta*k+(Age-1)*k)-EXP(k*to))^b-EXP(b*delta*k)*(EXP((Age-1)*k)-EXP(k*to))^b)*EXP(sigma_y*$Q26+sigma_c*N51+N73)</f>
+        <v>8.7448808905806832</v>
       </c>
       <c r="O27" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>7.7996632832375958</v>
+        <v>10.446716704345082</v>
       </c>
       <c r="Q27" s="3">
         <f t="shared" ca="1" si="18"/>
-        <v>0.72360492744873817</v>
+        <v>6.1047004149862125E-2</v>
       </c>
     </row>
     <row r="28" spans="5:17">
@@ -2574,47 +2582,47 @@
       </c>
       <c r="F28" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>4.8972582976464736E-2</v>
+        <v>4.1723951957346933E-2</v>
       </c>
       <c r="G28" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0.73099454250809259</v>
+        <v>0.78149689315865833</v>
       </c>
       <c r="H28" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>1.919459394447993</v>
+        <v>2.4821442862533165</v>
       </c>
       <c r="I28" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>3.6075216111354913</v>
+        <v>3.4483226543283152</v>
       </c>
       <c r="J28" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>5.1123703639529419</v>
+        <v>5.2341944643521812</v>
       </c>
       <c r="K28" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>6.1277706286523408</v>
+        <v>6.4420980045590852</v>
       </c>
       <c r="L28" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>7.1291297933015905</v>
+        <v>7.5588480213877025</v>
       </c>
       <c r="M28" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>6.9885499953427699</v>
+        <v>8.8395099025237549</v>
       </c>
       <c r="N28" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>7.5020946310070862</v>
+        <v>9.606267216058832</v>
       </c>
       <c r="O28" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>9.1879534366762456</v>
+        <v>9.1368355277178654</v>
       </c>
       <c r="Q28" s="3">
         <f t="shared" ca="1" si="18"/>
-        <v>0.14554064272576439</v>
+        <v>0.33961311120301746</v>
       </c>
     </row>
     <row r="29" spans="5:17">
@@ -2623,47 +2631,47 @@
       </c>
       <c r="F29" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>3.6692259681697155E-2</v>
+        <v>4.1760823750165064E-2</v>
       </c>
       <c r="G29" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0.74636352025104535</v>
+        <v>0.73182084208570752</v>
       </c>
       <c r="H29" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>2.0445656125443126</v>
+        <v>2.1567053785823038</v>
       </c>
       <c r="I29" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>3.2765242885135413</v>
+        <v>4.0042102980362779</v>
       </c>
       <c r="J29" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>5.3784970370804155</v>
+        <v>4.6919501177670702</v>
       </c>
       <c r="K29" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>6.4307491696122181</v>
+        <v>6.665254901354225</v>
       </c>
       <c r="L29" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>7.1009663054883276</v>
+        <v>7.44826188894198</v>
       </c>
       <c r="M29" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>7.8538301713597649</v>
+        <v>8.4652921014168108</v>
       </c>
       <c r="N29" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>7.5744180137530748</v>
+        <v>9.3923720880071393</v>
       </c>
       <c r="O29" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>7.840736356366703</v>
+        <v>10.10735867584569</v>
       </c>
       <c r="Q29" s="3">
         <f t="shared" ca="1" si="18"/>
-        <v>-1.906019015411242</v>
+        <v>1.1494252713786075</v>
       </c>
     </row>
     <row r="30" spans="5:17">
@@ -2672,47 +2680,47 @@
       </c>
       <c r="F30" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>3.067346879307721E-2</v>
+        <v>4.9599212598795822E-2</v>
       </c>
       <c r="G30" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0.62881896787481073</v>
+        <v>0.67345561513460817</v>
       </c>
       <c r="H30" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>1.9374994969180457</v>
+        <v>1.9999806476967159</v>
       </c>
       <c r="I30" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>3.4364527202092403</v>
+        <v>3.9969763867575256</v>
       </c>
       <c r="J30" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>4.1643758422040804</v>
+        <v>6.041517073603881</v>
       </c>
       <c r="K30" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>6.335683200910732</v>
+        <v>6.1027599698291413</v>
       </c>
       <c r="L30" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>7.2539023006251586</v>
+        <v>7.9310671831542123</v>
       </c>
       <c r="M30" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>7.7281405552735585</v>
+        <v>8.4370286769950997</v>
       </c>
       <c r="N30" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>8.4533585979368429</v>
+        <v>9.0168852117525606</v>
       </c>
       <c r="O30" s="1">
         <f t="shared" ca="1" si="17"/>
-        <v>7.8435354248664746</v>
+        <v>9.8324689288003313</v>
       </c>
       <c r="Q30" s="3">
         <f t="shared" ca="1" si="18"/>
-        <v>-3.1211283184982355</v>
+        <v>1.2731589590642622</v>
       </c>
     </row>
     <row r="35" spans="5:15">
@@ -2726,43 +2734,43 @@
       </c>
       <c r="F36" s="3">
         <f t="shared" ref="F36:F54" ca="1" si="19">_xlfn.NORM.INV(RAND(),0,1)</f>
-        <v>2.1828078220578297</v>
+        <v>0.83249681992498181</v>
       </c>
       <c r="G36" s="3">
         <f t="shared" ref="G36:O36" ca="1" si="20">_xlfn.NORM.INV(RAND(),0,1)</f>
-        <v>0.35693204233064801</v>
+        <v>0.16374810079559957</v>
       </c>
       <c r="H36" s="3">
         <f t="shared" ca="1" si="20"/>
-        <v>-1.7966083854482693</v>
+        <v>-1.0595694724853126</v>
       </c>
       <c r="I36" s="3">
         <f t="shared" ca="1" si="20"/>
-        <v>1.1017069874147833</v>
+        <v>-1.2220047451636322</v>
       </c>
       <c r="J36" s="3">
         <f t="shared" ca="1" si="20"/>
-        <v>-9.4948964756779483E-2</v>
+        <v>0.27361802512215561</v>
       </c>
       <c r="K36" s="3">
         <f t="shared" ca="1" si="20"/>
-        <v>0.42711412597084086</v>
+        <v>1.4969276633414299</v>
       </c>
       <c r="L36" s="3">
         <f t="shared" ca="1" si="20"/>
-        <v>-0.94244036298589873</v>
+        <v>-0.70495302876395749</v>
       </c>
       <c r="M36" s="3">
         <f t="shared" ca="1" si="20"/>
-        <v>0.29544627510701543</v>
+        <v>-0.91695682596392114</v>
       </c>
       <c r="N36" s="3">
         <f t="shared" ca="1" si="20"/>
-        <v>-0.4978562743750034</v>
+        <v>-0.95915361858617809</v>
       </c>
       <c r="O36" s="3">
         <f t="shared" ca="1" si="20"/>
-        <v>0.87812670820808858</v>
+        <v>0.96325204611296655</v>
       </c>
     </row>
     <row r="37" spans="5:15">
@@ -2771,43 +2779,43 @@
       </c>
       <c r="F37" s="3">
         <f t="shared" ca="1" si="19"/>
-        <v>-2.3447731764201416</v>
+        <v>0.59945234320569041</v>
       </c>
       <c r="G37" s="3">
         <f ca="1">F36</f>
-        <v>2.1828078220578297</v>
+        <v>0.83249681992498181</v>
       </c>
       <c r="H37" s="3">
         <f t="shared" ref="H37:O37" ca="1" si="21">G36</f>
-        <v>0.35693204233064801</v>
+        <v>0.16374810079559957</v>
       </c>
       <c r="I37" s="3">
         <f t="shared" ca="1" si="21"/>
-        <v>-1.7966083854482693</v>
+        <v>-1.0595694724853126</v>
       </c>
       <c r="J37" s="3">
         <f t="shared" ca="1" si="21"/>
-        <v>1.1017069874147833</v>
+        <v>-1.2220047451636322</v>
       </c>
       <c r="K37" s="3">
         <f t="shared" ca="1" si="21"/>
-        <v>-9.4948964756779483E-2</v>
+        <v>0.27361802512215561</v>
       </c>
       <c r="L37" s="3">
         <f t="shared" ca="1" si="21"/>
-        <v>0.42711412597084086</v>
+        <v>1.4969276633414299</v>
       </c>
       <c r="M37" s="3">
         <f t="shared" ca="1" si="21"/>
-        <v>-0.94244036298589873</v>
+        <v>-0.70495302876395749</v>
       </c>
       <c r="N37" s="3">
         <f t="shared" ca="1" si="21"/>
-        <v>0.29544627510701543</v>
+        <v>-0.91695682596392114</v>
       </c>
       <c r="O37" s="3">
         <f t="shared" ca="1" si="21"/>
-        <v>-0.4978562743750034</v>
+        <v>-0.95915361858617809</v>
       </c>
     </row>
     <row r="38" spans="5:15">
@@ -2816,43 +2824,43 @@
       </c>
       <c r="F38" s="3">
         <f t="shared" ca="1" si="19"/>
-        <v>0.36912884136577889</v>
+        <v>-1.2945030372851225E-2</v>
       </c>
       <c r="G38" s="3">
         <f t="shared" ref="G38:O54" ca="1" si="22">F37</f>
-        <v>-2.3447731764201416</v>
+        <v>0.59945234320569041</v>
       </c>
       <c r="H38" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>2.1828078220578297</v>
+        <v>0.83249681992498181</v>
       </c>
       <c r="I38" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>0.35693204233064801</v>
+        <v>0.16374810079559957</v>
       </c>
       <c r="J38" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.7966083854482693</v>
+        <v>-1.0595694724853126</v>
       </c>
       <c r="K38" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>1.1017069874147833</v>
+        <v>-1.2220047451636322</v>
       </c>
       <c r="L38" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-9.4948964756779483E-2</v>
+        <v>0.27361802512215561</v>
       </c>
       <c r="M38" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>0.42711412597084086</v>
+        <v>1.4969276633414299</v>
       </c>
       <c r="N38" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.94244036298589873</v>
+        <v>-0.70495302876395749</v>
       </c>
       <c r="O38" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>0.29544627510701543</v>
+        <v>-0.91695682596392114</v>
       </c>
     </row>
     <row r="39" spans="5:15">
@@ -2861,43 +2869,43 @@
       </c>
       <c r="F39" s="3">
         <f t="shared" ca="1" si="19"/>
-        <v>-9.2706295333680994E-2</v>
+        <v>-0.55332310270897545</v>
       </c>
       <c r="G39" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>0.36912884136577889</v>
+        <v>-1.2945030372851225E-2</v>
       </c>
       <c r="H39" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-2.3447731764201416</v>
+        <v>0.59945234320569041</v>
       </c>
       <c r="I39" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>2.1828078220578297</v>
+        <v>0.83249681992498181</v>
       </c>
       <c r="J39" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>0.35693204233064801</v>
+        <v>0.16374810079559957</v>
       </c>
       <c r="K39" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.7966083854482693</v>
+        <v>-1.0595694724853126</v>
       </c>
       <c r="L39" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>1.1017069874147833</v>
+        <v>-1.2220047451636322</v>
       </c>
       <c r="M39" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-9.4948964756779483E-2</v>
+        <v>0.27361802512215561</v>
       </c>
       <c r="N39" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>0.42711412597084086</v>
+        <v>1.4969276633414299</v>
       </c>
       <c r="O39" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.94244036298589873</v>
+        <v>-0.70495302876395749</v>
       </c>
     </row>
     <row r="40" spans="5:15">
@@ -2906,43 +2914,43 @@
       </c>
       <c r="F40" s="3">
         <f t="shared" ca="1" si="19"/>
-        <v>1.8264817934593671</v>
+        <v>0.23327471963978308</v>
       </c>
       <c r="G40" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-9.2706295333680994E-2</v>
+        <v>-0.55332310270897545</v>
       </c>
       <c r="H40" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>0.36912884136577889</v>
+        <v>-1.2945030372851225E-2</v>
       </c>
       <c r="I40" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-2.3447731764201416</v>
+        <v>0.59945234320569041</v>
       </c>
       <c r="J40" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>2.1828078220578297</v>
+        <v>0.83249681992498181</v>
       </c>
       <c r="K40" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>0.35693204233064801</v>
+        <v>0.16374810079559957</v>
       </c>
       <c r="L40" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.7966083854482693</v>
+        <v>-1.0595694724853126</v>
       </c>
       <c r="M40" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>1.1017069874147833</v>
+        <v>-1.2220047451636322</v>
       </c>
       <c r="N40" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-9.4948964756779483E-2</v>
+        <v>0.27361802512215561</v>
       </c>
       <c r="O40" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>0.42711412597084086</v>
+        <v>1.4969276633414299</v>
       </c>
     </row>
     <row r="41" spans="5:15">
@@ -2951,43 +2959,43 @@
       </c>
       <c r="F41" s="3">
         <f t="shared" ca="1" si="19"/>
-        <v>-1.1488110972138599</v>
+        <v>-1.3966963605228822</v>
       </c>
       <c r="G41" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>1.8264817934593671</v>
+        <v>0.23327471963978308</v>
       </c>
       <c r="H41" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-9.2706295333680994E-2</v>
+        <v>-0.55332310270897545</v>
       </c>
       <c r="I41" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>0.36912884136577889</v>
+        <v>-1.2945030372851225E-2</v>
       </c>
       <c r="J41" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-2.3447731764201416</v>
+        <v>0.59945234320569041</v>
       </c>
       <c r="K41" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>2.1828078220578297</v>
+        <v>0.83249681992498181</v>
       </c>
       <c r="L41" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>0.35693204233064801</v>
+        <v>0.16374810079559957</v>
       </c>
       <c r="M41" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.7966083854482693</v>
+        <v>-1.0595694724853126</v>
       </c>
       <c r="N41" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>1.1017069874147833</v>
+        <v>-1.2220047451636322</v>
       </c>
       <c r="O41" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-9.4948964756779483E-2</v>
+        <v>0.27361802512215561</v>
       </c>
     </row>
     <row r="42" spans="5:15">
@@ -2996,43 +3004,43 @@
       </c>
       <c r="F42" s="3">
         <f t="shared" ca="1" si="19"/>
-        <v>-1.6334609984439699</v>
+        <v>0.75190588128755209</v>
       </c>
       <c r="G42" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.1488110972138599</v>
+        <v>-1.3966963605228822</v>
       </c>
       <c r="H42" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>1.8264817934593671</v>
+        <v>0.23327471963978308</v>
       </c>
       <c r="I42" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-9.2706295333680994E-2</v>
+        <v>-0.55332310270897545</v>
       </c>
       <c r="J42" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>0.36912884136577889</v>
+        <v>-1.2945030372851225E-2</v>
       </c>
       <c r="K42" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-2.3447731764201416</v>
+        <v>0.59945234320569041</v>
       </c>
       <c r="L42" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>2.1828078220578297</v>
+        <v>0.83249681992498181</v>
       </c>
       <c r="M42" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>0.35693204233064801</v>
+        <v>0.16374810079559957</v>
       </c>
       <c r="N42" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.7966083854482693</v>
+        <v>-1.0595694724853126</v>
       </c>
       <c r="O42" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>1.1017069874147833</v>
+        <v>-1.2220047451636322</v>
       </c>
     </row>
     <row r="43" spans="5:15">
@@ -3041,43 +3049,43 @@
       </c>
       <c r="F43" s="3">
         <f t="shared" ca="1" si="19"/>
-        <v>-0.12657259079998209</v>
+        <v>0.10775680586326783</v>
       </c>
       <c r="G43" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.6334609984439699</v>
+        <v>0.75190588128755209</v>
       </c>
       <c r="H43" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.1488110972138599</v>
+        <v>-1.3966963605228822</v>
       </c>
       <c r="I43" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>1.8264817934593671</v>
+        <v>0.23327471963978308</v>
       </c>
       <c r="J43" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-9.2706295333680994E-2</v>
+        <v>-0.55332310270897545</v>
       </c>
       <c r="K43" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>0.36912884136577889</v>
+        <v>-1.2945030372851225E-2</v>
       </c>
       <c r="L43" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-2.3447731764201416</v>
+        <v>0.59945234320569041</v>
       </c>
       <c r="M43" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>2.1828078220578297</v>
+        <v>0.83249681992498181</v>
       </c>
       <c r="N43" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>0.35693204233064801</v>
+        <v>0.16374810079559957</v>
       </c>
       <c r="O43" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.7966083854482693</v>
+        <v>-1.0595694724853126</v>
       </c>
     </row>
     <row r="44" spans="5:15">
@@ -3086,43 +3094,43 @@
       </c>
       <c r="F44" s="3">
         <f t="shared" ca="1" si="19"/>
-        <v>-0.61225838409381339</v>
+        <v>1.2116753730095784</v>
       </c>
       <c r="G44" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.12657259079998209</v>
+        <v>0.10775680586326783</v>
       </c>
       <c r="H44" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.6334609984439699</v>
+        <v>0.75190588128755209</v>
       </c>
       <c r="I44" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.1488110972138599</v>
+        <v>-1.3966963605228822</v>
       </c>
       <c r="J44" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>1.8264817934593671</v>
+        <v>0.23327471963978308</v>
       </c>
       <c r="K44" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-9.2706295333680994E-2</v>
+        <v>-0.55332310270897545</v>
       </c>
       <c r="L44" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>0.36912884136577889</v>
+        <v>-1.2945030372851225E-2</v>
       </c>
       <c r="M44" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-2.3447731764201416</v>
+        <v>0.59945234320569041</v>
       </c>
       <c r="N44" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>2.1828078220578297</v>
+        <v>0.83249681992498181</v>
       </c>
       <c r="O44" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>0.35693204233064801</v>
+        <v>0.16374810079559957</v>
       </c>
     </row>
     <row r="45" spans="5:15">
@@ -3131,43 +3139,43 @@
       </c>
       <c r="F45" s="3">
         <f t="shared" ca="1" si="19"/>
-        <v>-0.88791785683197277</v>
+        <v>0.93851745912549334</v>
       </c>
       <c r="G45" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.61225838409381339</v>
+        <v>1.2116753730095784</v>
       </c>
       <c r="H45" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.12657259079998209</v>
+        <v>0.10775680586326783</v>
       </c>
       <c r="I45" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.6334609984439699</v>
+        <v>0.75190588128755209</v>
       </c>
       <c r="J45" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.1488110972138599</v>
+        <v>-1.3966963605228822</v>
       </c>
       <c r="K45" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>1.8264817934593671</v>
+        <v>0.23327471963978308</v>
       </c>
       <c r="L45" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-9.2706295333680994E-2</v>
+        <v>-0.55332310270897545</v>
       </c>
       <c r="M45" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>0.36912884136577889</v>
+        <v>-1.2945030372851225E-2</v>
       </c>
       <c r="N45" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-2.3447731764201416</v>
+        <v>0.59945234320569041</v>
       </c>
       <c r="O45" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>2.1828078220578297</v>
+        <v>0.83249681992498181</v>
       </c>
     </row>
     <row r="46" spans="5:15">
@@ -3176,43 +3184,43 @@
       </c>
       <c r="F46" s="3">
         <f t="shared" ca="1" si="19"/>
-        <v>4.2484761416153753E-2</v>
+        <v>0.67636639573342994</v>
       </c>
       <c r="G46" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.88791785683197277</v>
+        <v>0.93851745912549334</v>
       </c>
       <c r="H46" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.61225838409381339</v>
+        <v>1.2116753730095784</v>
       </c>
       <c r="I46" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.12657259079998209</v>
+        <v>0.10775680586326783</v>
       </c>
       <c r="J46" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.6334609984439699</v>
+        <v>0.75190588128755209</v>
       </c>
       <c r="K46" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.1488110972138599</v>
+        <v>-1.3966963605228822</v>
       </c>
       <c r="L46" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>1.8264817934593671</v>
+        <v>0.23327471963978308</v>
       </c>
       <c r="M46" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-9.2706295333680994E-2</v>
+        <v>-0.55332310270897545</v>
       </c>
       <c r="N46" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>0.36912884136577889</v>
+        <v>-1.2945030372851225E-2</v>
       </c>
       <c r="O46" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-2.3447731764201416</v>
+        <v>0.59945234320569041</v>
       </c>
     </row>
     <row r="47" spans="5:15">
@@ -3221,43 +3229,43 @@
       </c>
       <c r="F47" s="3">
         <f t="shared" ca="1" si="19"/>
-        <v>-2.2840055571224656E-2</v>
+        <v>0.31219264047583883</v>
       </c>
       <c r="G47" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>4.2484761416153753E-2</v>
+        <v>0.67636639573342994</v>
       </c>
       <c r="H47" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.88791785683197277</v>
+        <v>0.93851745912549334</v>
       </c>
       <c r="I47" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.61225838409381339</v>
+        <v>1.2116753730095784</v>
       </c>
       <c r="J47" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.12657259079998209</v>
+        <v>0.10775680586326783</v>
       </c>
       <c r="K47" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.6334609984439699</v>
+        <v>0.75190588128755209</v>
       </c>
       <c r="L47" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.1488110972138599</v>
+        <v>-1.3966963605228822</v>
       </c>
       <c r="M47" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>1.8264817934593671</v>
+        <v>0.23327471963978308</v>
       </c>
       <c r="N47" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-9.2706295333680994E-2</v>
+        <v>-0.55332310270897545</v>
       </c>
       <c r="O47" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>0.36912884136577889</v>
+        <v>-1.2945030372851225E-2</v>
       </c>
     </row>
     <row r="48" spans="5:15">
@@ -3266,43 +3274,43 @@
       </c>
       <c r="F48" s="3">
         <f t="shared" ca="1" si="19"/>
-        <v>-0.14213817613577032</v>
+        <v>0.61207800976445692</v>
       </c>
       <c r="G48" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-2.2840055571224656E-2</v>
+        <v>0.31219264047583883</v>
       </c>
       <c r="H48" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>4.2484761416153753E-2</v>
+        <v>0.67636639573342994</v>
       </c>
       <c r="I48" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.88791785683197277</v>
+        <v>0.93851745912549334</v>
       </c>
       <c r="J48" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.61225838409381339</v>
+        <v>1.2116753730095784</v>
       </c>
       <c r="K48" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.12657259079998209</v>
+        <v>0.10775680586326783</v>
       </c>
       <c r="L48" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.6334609984439699</v>
+        <v>0.75190588128755209</v>
       </c>
       <c r="M48" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.1488110972138599</v>
+        <v>-1.3966963605228822</v>
       </c>
       <c r="N48" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>1.8264817934593671</v>
+        <v>0.23327471963978308</v>
       </c>
       <c r="O48" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-9.2706295333680994E-2</v>
+        <v>-0.55332310270897545</v>
       </c>
     </row>
     <row r="49" spans="5:15">
@@ -3311,43 +3319,43 @@
       </c>
       <c r="F49" s="3">
         <f t="shared" ca="1" si="19"/>
-        <v>-0.41887045116956895</v>
+        <v>-0.32583082371486932</v>
       </c>
       <c r="G49" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.14213817613577032</v>
+        <v>0.61207800976445692</v>
       </c>
       <c r="H49" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-2.2840055571224656E-2</v>
+        <v>0.31219264047583883</v>
       </c>
       <c r="I49" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>4.2484761416153753E-2</v>
+        <v>0.67636639573342994</v>
       </c>
       <c r="J49" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.88791785683197277</v>
+        <v>0.93851745912549334</v>
       </c>
       <c r="K49" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.61225838409381339</v>
+        <v>1.2116753730095784</v>
       </c>
       <c r="L49" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.12657259079998209</v>
+        <v>0.10775680586326783</v>
       </c>
       <c r="M49" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.6334609984439699</v>
+        <v>0.75190588128755209</v>
       </c>
       <c r="N49" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.1488110972138599</v>
+        <v>-1.3966963605228822</v>
       </c>
       <c r="O49" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>1.8264817934593671</v>
+        <v>0.23327471963978308</v>
       </c>
     </row>
     <row r="50" spans="5:15">
@@ -3356,43 +3364,43 @@
       </c>
       <c r="F50" s="3">
         <f t="shared" ca="1" si="19"/>
-        <v>-1.7232975501885628</v>
+        <v>1.7970821548110039</v>
       </c>
       <c r="G50" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.41887045116956895</v>
+        <v>-0.32583082371486932</v>
       </c>
       <c r="H50" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.14213817613577032</v>
+        <v>0.61207800976445692</v>
       </c>
       <c r="I50" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-2.2840055571224656E-2</v>
+        <v>0.31219264047583883</v>
       </c>
       <c r="J50" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>4.2484761416153753E-2</v>
+        <v>0.67636639573342994</v>
       </c>
       <c r="K50" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.88791785683197277</v>
+        <v>0.93851745912549334</v>
       </c>
       <c r="L50" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.61225838409381339</v>
+        <v>1.2116753730095784</v>
       </c>
       <c r="M50" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.12657259079998209</v>
+        <v>0.10775680586326783</v>
       </c>
       <c r="N50" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.6334609984439699</v>
+        <v>0.75190588128755209</v>
       </c>
       <c r="O50" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.1488110972138599</v>
+        <v>-1.3966963605228822</v>
       </c>
     </row>
     <row r="51" spans="5:15">
@@ -3401,43 +3409,43 @@
       </c>
       <c r="F51" s="3">
         <f t="shared" ca="1" si="19"/>
-        <v>3.185458000963165E-2</v>
+        <v>0.97212014769359845</v>
       </c>
       <c r="G51" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.7232975501885628</v>
+        <v>1.7970821548110039</v>
       </c>
       <c r="H51" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.41887045116956895</v>
+        <v>-0.32583082371486932</v>
       </c>
       <c r="I51" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.14213817613577032</v>
+        <v>0.61207800976445692</v>
       </c>
       <c r="J51" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-2.2840055571224656E-2</v>
+        <v>0.31219264047583883</v>
       </c>
       <c r="K51" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>4.2484761416153753E-2</v>
+        <v>0.67636639573342994</v>
       </c>
       <c r="L51" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.88791785683197277</v>
+        <v>0.93851745912549334</v>
       </c>
       <c r="M51" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.61225838409381339</v>
+        <v>1.2116753730095784</v>
       </c>
       <c r="N51" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.12657259079998209</v>
+        <v>0.10775680586326783</v>
       </c>
       <c r="O51" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.6334609984439699</v>
+        <v>0.75190588128755209</v>
       </c>
     </row>
     <row r="52" spans="5:15">
@@ -3446,43 +3454,43 @@
       </c>
       <c r="F52" s="3">
         <f t="shared" ca="1" si="19"/>
-        <v>1.398837513907752</v>
+        <v>0.7842622655814</v>
       </c>
       <c r="G52" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>3.185458000963165E-2</v>
+        <v>0.97212014769359845</v>
       </c>
       <c r="H52" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.7232975501885628</v>
+        <v>1.7970821548110039</v>
       </c>
       <c r="I52" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.41887045116956895</v>
+        <v>-0.32583082371486932</v>
       </c>
       <c r="J52" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.14213817613577032</v>
+        <v>0.61207800976445692</v>
       </c>
       <c r="K52" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-2.2840055571224656E-2</v>
+        <v>0.31219264047583883</v>
       </c>
       <c r="L52" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>4.2484761416153753E-2</v>
+        <v>0.67636639573342994</v>
       </c>
       <c r="M52" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.88791785683197277</v>
+        <v>0.93851745912549334</v>
       </c>
       <c r="N52" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.61225838409381339</v>
+        <v>1.2116753730095784</v>
       </c>
       <c r="O52" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.12657259079998209</v>
+        <v>0.10775680586326783</v>
       </c>
     </row>
     <row r="53" spans="5:15">
@@ -3491,43 +3499,43 @@
       </c>
       <c r="F53" s="3">
         <f t="shared" ca="1" si="19"/>
-        <v>1.168679628222399</v>
+        <v>-2.1458814235989377E-2</v>
       </c>
       <c r="G53" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>1.398837513907752</v>
+        <v>0.7842622655814</v>
       </c>
       <c r="H53" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>3.185458000963165E-2</v>
+        <v>0.97212014769359845</v>
       </c>
       <c r="I53" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.7232975501885628</v>
+        <v>1.7970821548110039</v>
       </c>
       <c r="J53" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.41887045116956895</v>
+        <v>-0.32583082371486932</v>
       </c>
       <c r="K53" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.14213817613577032</v>
+        <v>0.61207800976445692</v>
       </c>
       <c r="L53" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-2.2840055571224656E-2</v>
+        <v>0.31219264047583883</v>
       </c>
       <c r="M53" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>4.2484761416153753E-2</v>
+        <v>0.67636639573342994</v>
       </c>
       <c r="N53" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.88791785683197277</v>
+        <v>0.93851745912549334</v>
       </c>
       <c r="O53" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.61225838409381339</v>
+        <v>1.2116753730095784</v>
       </c>
     </row>
     <row r="54" spans="5:15">
@@ -3536,43 +3544,43 @@
       </c>
       <c r="F54" s="3">
         <f t="shared" ca="1" si="19"/>
-        <v>-0.51790980395051078</v>
+        <v>1.6508280965889881</v>
       </c>
       <c r="G54" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>1.168679628222399</v>
+        <v>-2.1458814235989377E-2</v>
       </c>
       <c r="H54" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>1.398837513907752</v>
+        <v>0.7842622655814</v>
       </c>
       <c r="I54" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>3.185458000963165E-2</v>
+        <v>0.97212014769359845</v>
       </c>
       <c r="J54" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.7232975501885628</v>
+        <v>1.7970821548110039</v>
       </c>
       <c r="K54" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.41887045116956895</v>
+        <v>-0.32583082371486932</v>
       </c>
       <c r="L54" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.14213817613577032</v>
+        <v>0.61207800976445692</v>
       </c>
       <c r="M54" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-2.2840055571224656E-2</v>
+        <v>0.31219264047583883</v>
       </c>
       <c r="N54" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>4.2484761416153753E-2</v>
+        <v>0.67636639573342994</v>
       </c>
       <c r="O54" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-0.88791785683197277</v>
+        <v>0.93851745912549334</v>
       </c>
     </row>
     <row r="56" spans="5:15">
@@ -3631,43 +3639,43 @@
       </c>
       <c r="F58" s="6">
         <f t="shared" ref="F58:O67" ca="1" si="24">IF(cv_obs=0,0,_xlfn.NORM.INV(RAND(),0,sigma_obs))</f>
-        <v>-7.7414756041135013E-2</v>
+        <v>1.0872890575991771E-2</v>
       </c>
       <c r="G58" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-0.10861477058878358</v>
+        <v>-3.4113745279362916E-2</v>
       </c>
       <c r="H58" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>3.8520598646744945E-3</v>
+        <v>6.0186432619463069E-2</v>
       </c>
       <c r="I58" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>4.5798201612745032E-2</v>
+        <v>2.4668243783352549E-3</v>
       </c>
       <c r="J58" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>8.9251271433606283E-2</v>
+        <v>0.12967319372690514</v>
       </c>
       <c r="K58" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-3.5275104504981704E-2</v>
+        <v>0.11664254711037035</v>
       </c>
       <c r="L58" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-0.11527625747702198</v>
+        <v>8.0491245724165439E-2</v>
       </c>
       <c r="M58" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-0.13881273065720304</v>
+        <v>-5.5460924235639718E-2</v>
       </c>
       <c r="N58" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-3.8901725771388042E-2</v>
+        <v>1.6727683275101778E-2</v>
       </c>
       <c r="O58" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-1.368190864318982E-2</v>
+        <v>-4.3344301578796873E-2</v>
       </c>
     </row>
     <row r="59" spans="5:15">
@@ -3676,43 +3684,43 @@
       </c>
       <c r="F59" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>6.4671186068805389E-3</v>
+        <v>-3.4118097367226631E-2</v>
       </c>
       <c r="G59" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-9.8047688455364787E-4</v>
+        <v>-7.0763761903104946E-2</v>
       </c>
       <c r="H59" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>3.5006224132515633E-2</v>
+        <v>-5.1514119819811778E-2</v>
       </c>
       <c r="I59" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-8.8721924202250155E-2</v>
+        <v>-3.5544200015736785E-2</v>
       </c>
       <c r="J59" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-6.1406451401632464E-2</v>
+        <v>0.15388221508875022</v>
       </c>
       <c r="K59" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>0.19040715332171418</v>
+        <v>-4.2687557593291429E-3</v>
       </c>
       <c r="L59" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>0.18778864167705808</v>
+        <v>9.7224428878978503E-2</v>
       </c>
       <c r="M59" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>9.7863169564831459E-2</v>
+        <v>0.13615885960211122</v>
       </c>
       <c r="N59" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>0.23520957016040803</v>
+        <v>4.1986739338021606E-2</v>
       </c>
       <c r="O59" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-3.1122817840954969E-2</v>
+        <v>-9.1375592329560953E-2</v>
       </c>
     </row>
     <row r="60" spans="5:15">
@@ -3721,43 +3729,43 @@
       </c>
       <c r="F60" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>5.1925486819018318E-3</v>
+        <v>2.2100681644331509E-2</v>
       </c>
       <c r="G60" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>6.7996095632984005E-2</v>
+        <v>-6.0390228248451611E-2</v>
       </c>
       <c r="H60" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-2.6868303349787896E-2</v>
+        <v>-6.0981825127437474E-3</v>
       </c>
       <c r="I60" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>2.1077712864435239E-3</v>
+        <v>4.3281093153660591E-2</v>
       </c>
       <c r="J60" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>2.1884647014144418E-2</v>
+        <v>2.8155453583213818E-2</v>
       </c>
       <c r="K60" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>7.4956460997569085E-2</v>
+        <v>0.11206685870964393</v>
       </c>
       <c r="L60" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-0.12030851917156969</v>
+        <v>0.22332727335677832</v>
       </c>
       <c r="M60" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>2.5048923304333746E-4</v>
+        <v>0.12735572840054948</v>
       </c>
       <c r="N60" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-9.1491628959991647E-2</v>
+        <v>-6.3860459686603255E-2</v>
       </c>
       <c r="O60" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-0.10002661367654751</v>
+        <v>2.0563463644334172E-3</v>
       </c>
     </row>
     <row r="61" spans="5:15">
@@ -3766,43 +3774,43 @@
       </c>
       <c r="F61" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-7.0030590723951736E-2</v>
+        <v>2.3587717683003041E-2</v>
       </c>
       <c r="G61" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-7.9850686086320496E-2</v>
+        <v>-0.13396462410392673</v>
       </c>
       <c r="H61" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-8.6332658310241894E-2</v>
+        <v>-1.0221247189265117E-2</v>
       </c>
       <c r="I61" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-0.11407586406077086</v>
+        <v>9.2008703975088493E-2</v>
       </c>
       <c r="J61" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>0.10880817139162066</v>
+        <v>0.1750648623564541</v>
       </c>
       <c r="K61" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>6.2349053027695805E-2</v>
+        <v>7.9798002955912467E-2</v>
       </c>
       <c r="L61" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-9.0257882019264254E-2</v>
+        <v>0.12435189510415423</v>
       </c>
       <c r="M61" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>4.2083265383035438E-2</v>
+        <v>0.17434370924709278</v>
       </c>
       <c r="N61" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-6.9459731003343156E-2</v>
+        <v>0.17106387365525488</v>
       </c>
       <c r="O61" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-2.5670983808260241E-2</v>
+        <v>0.21122202707626153</v>
       </c>
     </row>
     <row r="62" spans="5:15">
@@ -3811,43 +3819,43 @@
       </c>
       <c r="F62" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>3.4693808888457398E-2</v>
+        <v>-3.5062132393528865E-2</v>
       </c>
       <c r="G62" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-4.4865983176281335E-2</v>
+        <v>2.7769345630247893E-2</v>
       </c>
       <c r="H62" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>0.12637241951961634</v>
+        <v>6.3635485739898384E-2</v>
       </c>
       <c r="I62" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>8.1994419457672191E-2</v>
+        <v>-2.253886390250413E-2</v>
       </c>
       <c r="J62" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>0.18261107407534799</v>
+        <v>-0.21628829335364078</v>
       </c>
       <c r="K62" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>8.8879123570066387E-2</v>
+        <v>-6.3025958551882102E-2</v>
       </c>
       <c r="L62" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>2.2785773124048059E-2</v>
+        <v>-3.7608613756389131E-2</v>
       </c>
       <c r="M62" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>3.2196790216338173E-2</v>
+        <v>8.7676714387096927E-2</v>
       </c>
       <c r="N62" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-0.10146826382380721</v>
+        <v>9.3497255009617697E-2</v>
       </c>
       <c r="O62" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-0.12484281294573077</v>
+        <v>9.530906843439492E-2</v>
       </c>
     </row>
     <row r="63" spans="5:15">
@@ -3856,43 +3864,43 @@
       </c>
       <c r="F63" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>5.9975615262425584E-3</v>
+        <v>-2.2474814590883962E-3</v>
       </c>
       <c r="G63" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>1.9178514994581081E-2</v>
+        <v>3.4392660048396073E-3</v>
       </c>
       <c r="H63" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-7.1373452123763854E-3</v>
+        <v>1.0104353155692764E-2</v>
       </c>
       <c r="I63" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>1.5703937235256777E-2</v>
+        <v>6.1326572951651816E-2</v>
       </c>
       <c r="J63" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-7.9531378039050041E-2</v>
+        <v>-4.6354088713312008E-2</v>
       </c>
       <c r="K63" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-4.3189918229918141E-2</v>
+        <v>-0.18289014111532348</v>
       </c>
       <c r="L63" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-2.3181541663483064E-2</v>
+        <v>-0.11669121477749418</v>
       </c>
       <c r="M63" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>0.10363717375244585</v>
+        <v>-3.7247809006756664E-3</v>
       </c>
       <c r="N63" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>1.8422834247072591E-2</v>
+        <v>-0.15558840542849961</v>
       </c>
       <c r="O63" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>0.14239255656964758</v>
+        <v>0.17542253722245787</v>
       </c>
     </row>
     <row r="64" spans="5:15">
@@ -3901,43 +3909,43 @@
       </c>
       <c r="F64" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-8.339614102543717E-3</v>
+        <v>5.2761116259881946E-2</v>
       </c>
       <c r="G64" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-6.694584526783133E-2</v>
+        <v>-1.087498277444795E-2</v>
       </c>
       <c r="H64" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>1.8081624322652153E-2</v>
+        <v>5.298861270165315E-2</v>
       </c>
       <c r="I64" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-1.391480148493348E-2</v>
+        <v>0.1356814264107363</v>
       </c>
       <c r="J64" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-3.8873163635547166E-2</v>
+        <v>4.8618884359631978E-3</v>
       </c>
       <c r="K64" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>1.6812132768617465E-2</v>
+        <v>6.4823891218182883E-2</v>
       </c>
       <c r="L64" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>0.14424165354216498</v>
+        <v>2.9928019933886142E-2</v>
       </c>
       <c r="M64" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-5.7318499999986845E-2</v>
+        <v>1.7556953592688382E-3</v>
       </c>
       <c r="N64" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>7.8056553426096159E-2</v>
+        <v>-1.9294901081639747E-2</v>
       </c>
       <c r="O64" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-0.16792275695132333</v>
+        <v>-4.2066485170051973E-2</v>
       </c>
     </row>
     <row r="65" spans="5:15">
@@ -3946,43 +3954,43 @@
       </c>
       <c r="F65" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>6.0916367928287841E-2</v>
+        <v>7.9572789578456468E-2</v>
       </c>
       <c r="G65" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>4.1712167267123165E-2</v>
+        <v>8.8153937030057538E-3</v>
       </c>
       <c r="H65" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>3.4469210801481485E-2</v>
+        <v>-4.286660927113764E-2</v>
       </c>
       <c r="I65" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-6.7176245042420799E-2</v>
+        <v>-2.9866646486039358E-2</v>
       </c>
       <c r="J65" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-5.7714316838914523E-2</v>
+        <v>-4.6060723822739402E-2</v>
       </c>
       <c r="K65" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>6.9792664374957319E-2</v>
+        <v>0.13317129747989462</v>
       </c>
       <c r="L65" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>6.7973233781652903E-2</v>
+        <v>0.15897578972433565</v>
       </c>
       <c r="M65" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>5.7676857728576593E-2</v>
+        <v>-0.26107488122923994</v>
       </c>
       <c r="N65" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-4.4973409217568129E-2</v>
+        <v>-0.26330689251506906</v>
       </c>
       <c r="O65" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-2.657921465268414E-2</v>
+        <v>-1.7177723460314844E-2</v>
       </c>
     </row>
     <row r="66" spans="5:15">
@@ -3991,43 +3999,43 @@
       </c>
       <c r="F66" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>1.5201703273164245E-2</v>
+        <v>-1.2508232019060881E-3</v>
       </c>
       <c r="G66" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-1.1812181406198444E-2</v>
+        <v>-1.3300553625680646E-2</v>
       </c>
       <c r="H66" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>1.9463438558479436E-2</v>
+        <v>6.3865534644913569E-2</v>
       </c>
       <c r="I66" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>0.1553821163441825</v>
+        <v>-3.3175293186572377E-2</v>
       </c>
       <c r="J66" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-9.7754666202008955E-2</v>
+        <v>1.4032897298896225E-2</v>
       </c>
       <c r="K66" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>2.1909833617821506E-2</v>
+        <v>-0.12786154310245632</v>
       </c>
       <c r="L66" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>5.2857527270044946E-2</v>
+        <v>0.141664307801461</v>
       </c>
       <c r="M66" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-5.938937409290674E-2</v>
+        <v>0.2063276528267059</v>
       </c>
       <c r="N66" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>0.16718706008648651</v>
+        <v>-0.10194830447454499</v>
       </c>
       <c r="O66" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>0.20523206919632825</v>
+        <v>0.16067722241390545</v>
       </c>
     </row>
     <row r="67" spans="5:15">
@@ -4036,43 +4044,43 @@
       </c>
       <c r="F67" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>2.6143983516377901E-2</v>
+        <v>-4.9131866800139366E-3</v>
       </c>
       <c r="G67" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-5.1062070511261187E-2</v>
+        <v>1.9729052631731823E-2</v>
       </c>
       <c r="H67" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>2.9514450596471054E-2</v>
+        <v>4.1353762044759566E-2</v>
       </c>
       <c r="I67" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>9.5896657861324133E-2</v>
+        <v>-1.4187698133687313E-2</v>
       </c>
       <c r="J67" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-6.394786766206622E-3</v>
+        <v>4.0444168116579193E-2</v>
       </c>
       <c r="K67" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>8.257114576811514E-2</v>
+        <v>-2.9290496995127452E-2</v>
       </c>
       <c r="L67" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>3.5848736977985955E-2</v>
+        <v>-0.17260256789993952</v>
       </c>
       <c r="M67" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-0.30104764907385895</v>
+        <v>-0.1239319425877423</v>
       </c>
       <c r="N67" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-6.1680528718955116E-2</v>
+        <v>3.8098906578306675E-2</v>
       </c>
       <c r="O67" s="6">
         <f t="shared" ca="1" si="24"/>
-        <v>-0.19960959822609572</v>
+        <v>0.10375134133887634</v>
       </c>
     </row>
     <row r="68" spans="5:15">
@@ -4081,43 +4089,43 @@
       </c>
       <c r="F68" s="6">
         <f t="shared" ref="F68:O76" ca="1" si="25">IF(cv_obs=0,0,_xlfn.NORM.INV(RAND(),0,sigma_obs))</f>
-        <v>2.844400749182446E-2</v>
+        <v>1.6871858827031926E-2</v>
       </c>
       <c r="G68" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-5.4720582154065374E-3</v>
+        <v>7.8629570309081659E-2</v>
       </c>
       <c r="H68" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-7.3009557727795771E-2</v>
+        <v>3.2003128362409809E-2</v>
       </c>
       <c r="I68" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>0.11435038431574135</v>
+        <v>-3.4974886722179445E-2</v>
       </c>
       <c r="J68" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-5.3470101066870952E-2</v>
+        <v>0.11033270532696884</v>
       </c>
       <c r="K68" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.29108557795676288</v>
+        <v>-3.303791957590705E-2</v>
       </c>
       <c r="L68" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.18344620061357778</v>
+        <v>-0.25720627566897636</v>
       </c>
       <c r="M68" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.11733995699259801</v>
+        <v>6.7407425680927141E-2</v>
       </c>
       <c r="N68" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.1032979582973815</v>
+        <v>0.32236606243823435</v>
       </c>
       <c r="O68" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.33386331084437182</v>
+        <v>-0.1497432185482038</v>
       </c>
     </row>
     <row r="69" spans="5:15">
@@ -4126,43 +4134,43 @@
       </c>
       <c r="F69" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-7.8241861977846577E-2</v>
+        <v>-5.6659953009887437E-2</v>
       </c>
       <c r="G69" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>1.4519531359030955E-2</v>
+        <v>1.5169305587402768E-2</v>
       </c>
       <c r="H69" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>1.8171007375946364E-2</v>
+        <v>4.8766092747178469E-2</v>
       </c>
       <c r="I69" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-2.4897269756151912E-2</v>
+        <v>-6.688351090956811E-3</v>
       </c>
       <c r="J69" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-5.5907272878362606E-2</v>
+        <v>8.7832572787883645E-2</v>
       </c>
       <c r="K69" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.10488870594511067</v>
+        <v>4.6647559598096855E-2</v>
       </c>
       <c r="L69" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>7.548434569227129E-2</v>
+        <v>5.6075375723563463E-2</v>
       </c>
       <c r="M69" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-3.1533492320710385E-2</v>
+        <v>-9.5448524655288206E-2</v>
       </c>
       <c r="N69" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-6.6525654008565582E-2</v>
+        <v>0.16934391845980462</v>
       </c>
       <c r="O69" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-3.5931199627671465E-3</v>
+        <v>-0.29414382784544024</v>
       </c>
     </row>
     <row r="70" spans="5:15">
@@ -4171,43 +4179,43 @@
       </c>
       <c r="F70" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>1.6356659199098744E-2</v>
+        <v>8.0248936403189544E-2</v>
       </c>
       <c r="G70" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-7.6745928998894972E-2</v>
+        <v>-4.0615678041167183E-2</v>
       </c>
       <c r="H70" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-3.2523717678509668E-3</v>
+        <v>-8.3686938206326278E-2</v>
       </c>
       <c r="I70" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-6.0243816220985388E-2</v>
+        <v>-3.1521825404891055E-2</v>
       </c>
       <c r="J70" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.12028660359480996</v>
+        <v>-1.1772582957550948E-2</v>
       </c>
       <c r="K70" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-2.2790665501580602E-2</v>
+        <v>-2.7971006884818003E-2</v>
       </c>
       <c r="L70" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.11603676387417171</v>
+        <v>2.7589935511008402E-2</v>
       </c>
       <c r="M70" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>4.9774182373233611E-2</v>
+        <v>6.4434648792513136E-2</v>
       </c>
       <c r="N70" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>0.18105872127015885</v>
+        <v>3.0379400203446406E-2</v>
       </c>
       <c r="O70" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>0.27656164669986533</v>
+        <v>0.21518624057340505</v>
       </c>
     </row>
     <row r="71" spans="5:15">
@@ -4216,43 +4224,43 @@
       </c>
       <c r="F71" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-2.5097954402579222E-2</v>
+        <v>-1.957341007907051E-2</v>
       </c>
       <c r="G71" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>5.2615734091985181E-2</v>
+        <v>-2.7497694564983632E-2</v>
       </c>
       <c r="H71" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>2.9104453907718122E-2</v>
+        <v>0.10465661873821766</v>
       </c>
       <c r="I71" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-4.5996176405642526E-2</v>
+        <v>-6.1862824343361447E-2</v>
       </c>
       <c r="J71" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.11465981947347581</v>
+        <v>-8.2664800369069882E-2</v>
       </c>
       <c r="K71" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.14995444483620624</v>
+        <v>1.155096788018975E-2</v>
       </c>
       <c r="L71" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>3.8775024059102853E-2</v>
+        <v>5.3072998892810641E-2</v>
       </c>
       <c r="M71" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-8.4566934034934774E-2</v>
+        <v>0.19421451491247524</v>
       </c>
       <c r="N71" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.22615225986950327</v>
+        <v>-7.977755682041085E-2</v>
       </c>
       <c r="O71" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-9.6690680906453885E-2</v>
+        <v>-4.5921318126472425E-2</v>
       </c>
     </row>
     <row r="72" spans="5:15">
@@ -4261,43 +4269,43 @@
       </c>
       <c r="F72" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-7.8218507802331472E-4</v>
+        <v>1.7257227100647376E-2</v>
       </c>
       <c r="G72" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>2.680752179792709E-2</v>
+        <v>2.0855241417899257E-2</v>
       </c>
       <c r="H72" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>0.10735317777694892</v>
+        <v>-2.5695286669206761E-2</v>
       </c>
       <c r="I72" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>4.2585656681926161E-2</v>
+        <v>5.7720790824754557E-2</v>
       </c>
       <c r="J72" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>7.0382340812389393E-2</v>
+        <v>3.9609684168031296E-2</v>
       </c>
       <c r="K72" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-4.6102956672231341E-2</v>
+        <v>0.22142334276695444</v>
       </c>
       <c r="L72" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-8.6989403644749289E-2</v>
+        <v>-6.947288842161907E-2</v>
       </c>
       <c r="M72" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.10295843381388947</v>
+        <v>-2.2050630701039776E-2</v>
       </c>
       <c r="N72" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>7.886542821054579E-2</v>
+        <v>0.16521424567809875</v>
       </c>
       <c r="O72" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.25103111863803024</v>
+        <v>3.7597090374420604E-4</v>
       </c>
     </row>
     <row r="73" spans="5:15">
@@ -4306,43 +4314,43 @@
       </c>
       <c r="F73" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-3.3173831255509122E-2</v>
+        <v>1.0733898212461419E-2</v>
       </c>
       <c r="G73" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>9.3613929410460123E-2</v>
+        <v>1.0470251595911702E-2</v>
       </c>
       <c r="H73" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-5.232415128094986E-2</v>
+        <v>-2.852473854768528E-2</v>
       </c>
       <c r="I73" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-4.8573593756856076E-2</v>
+        <v>-7.8963959333750347E-2</v>
       </c>
       <c r="J73" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>3.211985212570783E-2</v>
+        <v>-6.6709778529136801E-2</v>
       </c>
       <c r="K73" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.17009700550454204</v>
+        <v>2.4653195268573371E-2</v>
       </c>
       <c r="L73" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-1.9957165599535913E-2</v>
+        <v>-8.2928486543673838E-2</v>
       </c>
       <c r="M73" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.19154564610985284</v>
+        <v>-4.7869987188605842E-2</v>
       </c>
       <c r="N73" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>6.8697884656783925E-3</v>
+        <v>-5.2402953672813272E-2</v>
       </c>
       <c r="O73" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>0.19117616935212814</v>
+        <v>0.28571865942245617</v>
       </c>
     </row>
     <row r="74" spans="5:15">
@@ -4351,43 +4359,43 @@
       </c>
       <c r="F74" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>1.4063189453224515E-2</v>
+        <v>-7.0110480489927282E-2</v>
       </c>
       <c r="G74" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-3.5069482113230461E-3</v>
+        <v>4.1709402158766777E-2</v>
       </c>
       <c r="H74" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>8.5891844904303932E-2</v>
+        <v>6.2143226933313513E-2</v>
       </c>
       <c r="I74" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>0.11870045820699272</v>
+        <v>4.0643092495008873E-2</v>
       </c>
       <c r="J74" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>1.9297220125241928E-2</v>
+        <v>6.6466500659877539E-2</v>
       </c>
       <c r="K74" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.14172534571098294</v>
+        <v>-8.3630385268550378E-2</v>
       </c>
       <c r="L74" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>0.1022534870720636</v>
+        <v>-6.4162668014273866E-2</v>
       </c>
       <c r="M74" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>3.9247210654970874E-2</v>
+        <v>-0.16544149207711578</v>
       </c>
       <c r="N74" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>7.0703705925715121E-2</v>
+        <v>4.2456003707935092E-2</v>
       </c>
       <c r="O74" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>0.12304206877360192</v>
+        <v>-6.4909930666444043E-2</v>
       </c>
     </row>
     <row r="75" spans="5:15">
@@ -4396,43 +4404,43 @@
       </c>
       <c r="F75" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-4.6459841625999816E-2</v>
+        <v>1.1344945316003843E-2</v>
       </c>
       <c r="G75" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-6.8587337971372286E-2</v>
+        <v>-3.0898797963095515E-3</v>
       </c>
       <c r="H75" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-8.5568022959483514E-3</v>
+        <v>-4.2173385458671525E-2</v>
       </c>
       <c r="I75" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>3.1562708906902139E-2</v>
+        <v>-0.19117676850805779</v>
       </c>
       <c r="J75" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>0.21765856482987309</v>
+        <v>-0.13058933376117002</v>
       </c>
       <c r="K75" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>5.7371042367617156E-2</v>
+        <v>7.8516417596806054E-2</v>
       </c>
       <c r="L75" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-3.0569650199384513E-2</v>
+        <v>-1.6203779882592698E-2</v>
       </c>
       <c r="M75" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-6.3972232024702133E-2</v>
+        <v>0.11096471153961895</v>
       </c>
       <c r="N75" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>0.11052346928406746</v>
+        <v>-0.1155517797371674</v>
       </c>
       <c r="O75" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.15366589628203156</v>
+        <v>7.0340740002153693E-2</v>
       </c>
     </row>
     <row r="76" spans="5:15">
@@ -4441,43 +4449,43 @@
       </c>
       <c r="F76" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>6.4542279194296712E-2</v>
+        <v>1.6132543616139899E-2</v>
       </c>
       <c r="G76" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-4.041076636480582E-3</v>
+        <v>-1.0943427547331748E-2</v>
       </c>
       <c r="H76" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-3.794111190447147E-2</v>
+        <v>-0.1044260648989714</v>
       </c>
       <c r="I76" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>8.6539718085684142E-2</v>
+        <v>8.1163649795182216E-2</v>
       </c>
       <c r="J76" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.13722396158317476</v>
+        <v>0.1507156131660575</v>
       </c>
       <c r="K76" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-2.9959946443686266E-2</v>
+        <v>0.15805546983008059</v>
       </c>
       <c r="L76" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>1.9073206770154675E-2</v>
+        <v>0.18337675394628189</v>
       </c>
       <c r="M76" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>3.1823300634849713E-3</v>
+        <v>0.23431124455674107</v>
       </c>
       <c r="N76" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>0.24568802410475477</v>
+        <v>-9.1634775839891894E-2</v>
       </c>
       <c r="O76" s="6">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.15073891744525311</v>
+        <v>-3.213731209078946E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>